<commit_message>
Created dataset and matlab script for processing Electric potential in the cell
</commit_message>
<xml_diff>
--- a/data/Couedel_PhysRevE_105_015210_fig08.xlsx
+++ b/data/Couedel_PhysRevE_105_015210_fig08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgeaugustomartinezortiz/Documents/Github/VDRIAD/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6EF65C-4FC3-5640-988A-DED838B28E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554824FB-1160-FC44-A7F3-8B9014FBC58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="12560" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -896,7 +896,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -929,11 +929,11 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E2">
         <f>D2-150</f>
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -983,11 +983,11 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated Excel spreadsheets to reflect correct information
</commit_message>
<xml_diff>
--- a/data/Couedel_PhysRevE_105_015210_fig08.xlsx
+++ b/data/Couedel_PhysRevE_105_015210_fig08.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgeaugustomartinezortiz/Documents/Github/VDRIAD/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554824FB-1160-FC44-A7F3-8B9014FBC58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFF6AAC-9E8A-E642-8AA3-83D2A01CA16D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="12560" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21540" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Couedel_PhysRevE_105_015210_fig" sheetId="1" r:id="rId1"/>
@@ -534,10 +534,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -893,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -919,349 +917,331 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2">
         <v>0.5</v>
       </c>
-      <c r="B2" s="2">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>40.4</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E19" si="0">(D2-10) * (50/10.6) - 150</f>
+        <v>-6.6037735849056673</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.5</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>38</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>-17.924528301886795</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0.5</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>-31.132075471698087</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0.5</v>
+      </c>
+      <c r="B5">
+        <v>25</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>38.6</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>-15.094339622641485</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0.5</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>34.4</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>-34.905660377358487</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0.5</v>
+      </c>
+      <c r="B7">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>29.4</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>-58.490566037735846</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>37.6</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>-19.811320754716974</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>35.4</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>-30.188679245283012</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>31.8</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>-47.169811320754704</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>-37.735849056603783</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>28</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>-65.094339622641499</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>21.2</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>-97.169811320754718</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1.5</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>-21.698113207547152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1.5</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>33.6</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>-38.679245283018858</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1.5</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>29.2</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>-59.433962264150935</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1.5</v>
+      </c>
+      <c r="B17">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>30.6</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>-52.830188679245268</v>
+      </c>
+      <c r="F17" t="s">
         <v>2</v>
       </c>
-      <c r="D2">
-        <v>161</v>
-      </c>
-      <c r="E2">
-        <f>D2-150</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="B3" s="2">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>146</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E19" si="0">D3-150</f>
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="B4" s="2">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1.5</v>
+      </c>
+      <c r="B18">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>23.6</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>-85.849056603773576</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1.5</v>
+      </c>
+      <c r="B19">
+        <v>25</v>
+      </c>
+      <c r="C19">
         <v>6</v>
       </c>
-      <c r="D4">
-        <v>124</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>-26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>25</v>
-      </c>
-      <c r="C5" s="2">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>165</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>25</v>
-      </c>
-      <c r="C6" s="2">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>136</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>-14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="B7" s="2">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>94</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>-56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>1</v>
-      </c>
-      <c r="B8" s="2">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>158</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>1</v>
-      </c>
-      <c r="B9" s="2">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>138</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2">
-        <v>6</v>
-      </c>
-      <c r="D10">
-        <v>105</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>-45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2">
-        <v>25</v>
-      </c>
-      <c r="C11" s="2">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>155</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2">
-        <v>25</v>
-      </c>
-      <c r="C12" s="2">
-        <v>4</v>
-      </c>
-      <c r="D12">
-        <v>115</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>-35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>1</v>
-      </c>
-      <c r="B13" s="2">
-        <v>25</v>
-      </c>
-      <c r="C13" s="2">
-        <v>6</v>
-      </c>
-      <c r="D13">
-        <v>55</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>-95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="B14" s="2">
-        <v>5</v>
-      </c>
-      <c r="C14" s="2">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>156</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="B15" s="2">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2">
-        <v>4</v>
-      </c>
-      <c r="D15">
-        <v>131</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="B16" s="2">
-        <v>5</v>
-      </c>
-      <c r="C16" s="2">
-        <v>6</v>
-      </c>
-      <c r="D16">
-        <v>92</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>-58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="B17" s="2">
-        <v>25</v>
-      </c>
-      <c r="C17" s="2">
-        <v>2</v>
-      </c>
-      <c r="D17">
-        <v>150</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="B18" s="2">
-        <v>25</v>
-      </c>
-      <c r="C18" s="2">
-        <v>4</v>
-      </c>
-      <c r="D18">
-        <v>99</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>-51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="B19" s="2">
-        <v>25</v>
-      </c>
-      <c r="C19" s="2">
-        <v>6</v>
-      </c>
       <c r="D19">
-        <v>25</v>
+        <v>15.2</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>-125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C24" s="1"/>
-      <c r="F24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C25" s="1"/>
+        <v>-125.47169811320755</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>